<commit_message>
Progess with Dr. Miller's help
</commit_message>
<xml_diff>
--- a/data/MasterGlutamateSpreadsheet.xlsx
+++ b/data/MasterGlutamateSpreadsheet.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10788" windowHeight="8262" activeTab="2" xr2:uid="{76EBCDB3-6D80-4011-A7B4-774B8706190D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10788" windowHeight="8262" xr2:uid="{76EBCDB3-6D80-4011-A7B4-774B8706190D}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeControl" sheetId="1" r:id="rId1"/>
-    <sheet name="1mMGlu" sheetId="2" r:id="rId2"/>
-    <sheet name="3mMGlu" sheetId="3" r:id="rId3"/>
+    <sheet name="Glu1mM" sheetId="2" r:id="rId2"/>
+    <sheet name="Glu3mM" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -34,51 +34,6 @@
     <t>Age</t>
   </si>
   <si>
-    <t>m1r1</t>
-  </si>
-  <si>
-    <t>m1r2</t>
-  </si>
-  <si>
-    <t>m1r3</t>
-  </si>
-  <si>
-    <t>m1r4</t>
-  </si>
-  <si>
-    <t>m1r5</t>
-  </si>
-  <si>
-    <t>m1r6</t>
-  </si>
-  <si>
-    <t>m2r1</t>
-  </si>
-  <si>
-    <t>m2r2</t>
-  </si>
-  <si>
-    <t>m2r3</t>
-  </si>
-  <si>
-    <t>m2r4</t>
-  </si>
-  <si>
-    <t>m2r5</t>
-  </si>
-  <si>
-    <t>m2r6</t>
-  </si>
-  <si>
-    <t>m3r1</t>
-  </si>
-  <si>
-    <t>m3r2</t>
-  </si>
-  <si>
-    <t>m3r3</t>
-  </si>
-  <si>
     <t>Dose</t>
   </si>
   <si>
@@ -86,15 +41,6 @@
   </si>
   <si>
     <t>FST</t>
-  </si>
-  <si>
-    <t>m3r4</t>
-  </si>
-  <si>
-    <t>m3r5</t>
-  </si>
-  <si>
-    <t>m3r6</t>
   </si>
   <si>
     <t>DOB</t>
@@ -127,13 +73,67 @@
     <t>NA</t>
   </si>
   <si>
-    <t>TimePosition</t>
-  </si>
-  <si>
     <t>G20</t>
   </si>
   <si>
     <t>3mM_glu</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>T0</t>
+  </si>
+  <si>
+    <t>T3.5</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>T10.5</t>
+  </si>
+  <si>
+    <t>T14</t>
+  </si>
+  <si>
+    <t>T17.5</t>
+  </si>
+  <si>
+    <t>T21</t>
+  </si>
+  <si>
+    <t>T24.5</t>
+  </si>
+  <si>
+    <t>T28</t>
+  </si>
+  <si>
+    <t>T31.5</t>
+  </si>
+  <si>
+    <t>T35</t>
+  </si>
+  <si>
+    <t>T38.5</t>
+  </si>
+  <si>
+    <t>T42</t>
+  </si>
+  <si>
+    <t>T45.5</t>
+  </si>
+  <si>
+    <t>T49</t>
+  </si>
+  <si>
+    <t>T52.5</t>
+  </si>
+  <si>
+    <t>T56</t>
+  </si>
+  <si>
+    <t>T59.5</t>
   </si>
 </sst>
 </file>
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FCD8EB7-4592-4D74-BEC1-FD73B58EE5E9}">
   <dimension ref="A1:AB31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -507,88 +507,88 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+      <c r="S1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" t="s">
+      <c r="T1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="U1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="V1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z1" t="s">
         <v>33</v>
       </c>
-      <c r="K1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>8</v>
-      </c>
-      <c r="R1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S1" t="s">
-        <v>10</v>
-      </c>
-      <c r="T1" t="s">
-        <v>11</v>
-      </c>
-      <c r="U1" t="s">
-        <v>12</v>
-      </c>
-      <c r="V1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W1" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>20</v>
-      </c>
       <c r="AA1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="AB1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.55000000000000004">
@@ -603,10 +603,10 @@
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K2">
         <v>33.101272340000001</v>
@@ -675,10 +675,10 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K3">
         <v>12.76035802</v>
@@ -747,10 +747,10 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K4">
         <v>46.098958969999998</v>
@@ -819,10 +819,10 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K5">
         <v>24.355979999999999</v>
@@ -891,10 +891,10 @@
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J6" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K6">
         <v>32.165161609999998</v>
@@ -963,10 +963,10 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J7" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K7">
         <v>22.905249999999999</v>
@@ -1035,10 +1035,10 @@
         <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K8">
         <v>26.288089020000001</v>
@@ -1107,10 +1107,10 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J9" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K9">
         <v>17.943367246000001</v>
@@ -1179,10 +1179,10 @@
         <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J10" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K10">
         <v>21.224036833700001</v>
@@ -1251,10 +1251,10 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J11" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K11">
         <v>34.632897027699997</v>
@@ -1323,10 +1323,10 @@
         <v>2</v>
       </c>
       <c r="I12" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J12" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K12">
         <v>45.996479035555552</v>
@@ -1395,10 +1395,10 @@
         <v>2</v>
       </c>
       <c r="I13" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J13" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K13">
         <v>16.430493673333334</v>
@@ -1467,10 +1467,10 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J14" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K14">
         <v>60.988059410000005</v>
@@ -1539,10 +1539,10 @@
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J15" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K15">
         <v>37.457593917499999</v>
@@ -1611,10 +1611,10 @@
         <v>2</v>
       </c>
       <c r="I16" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J16" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K16">
         <v>39.087522507499997</v>
@@ -1683,10 +1683,10 @@
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J17" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K17">
         <v>32.521394093333335</v>
@@ -1755,10 +1755,10 @@
         <v>2</v>
       </c>
       <c r="I18" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J18" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K18">
         <v>32.928235190000002</v>
@@ -1827,10 +1827,10 @@
         <v>1</v>
       </c>
       <c r="I19" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J19" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K19">
         <v>21.9571186963</v>
@@ -1899,10 +1899,10 @@
         <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J20" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K20">
         <v>26.7380866749</v>
@@ -1971,10 +1971,10 @@
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J21" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K21">
         <v>49.345949804299998</v>
@@ -2043,10 +2043,10 @@
         <v>2</v>
       </c>
       <c r="I22" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J22" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K22">
         <v>69.930069000000003</v>
@@ -2115,10 +2115,10 @@
         <v>2</v>
       </c>
       <c r="I23" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J23" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K23">
         <v>30.959752999999999</v>
@@ -2187,10 +2187,10 @@
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J24" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K24">
         <v>128.20512400000001</v>
@@ -2259,10 +2259,10 @@
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J25" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K25">
         <v>57.306590999999997</v>
@@ -2331,10 +2331,10 @@
         <v>2</v>
       </c>
       <c r="I26" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J26" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K26">
         <v>51.150894200000003</v>
@@ -2403,10 +2403,10 @@
         <v>1</v>
       </c>
       <c r="I27" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J27" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K27">
         <v>55.248619099999999</v>
@@ -2475,10 +2475,10 @@
         <v>2</v>
       </c>
       <c r="I28" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J28" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K28">
         <v>41.152263640000001</v>
@@ -2547,10 +2547,10 @@
         <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J29" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K29">
         <v>37.105751040000001</v>
@@ -2619,10 +2619,10 @@
         <v>2</v>
       </c>
       <c r="I30" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J30" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K30">
         <v>41.32231522</v>
@@ -2691,10 +2691,10 @@
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J31" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K31">
         <v>86.580085749999995</v>
@@ -2761,7 +2761,7 @@
   <dimension ref="A1:AB37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2773,88 +2773,88 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+      <c r="S1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" t="s">
+      <c r="T1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="U1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="V1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z1" t="s">
         <v>33</v>
       </c>
-      <c r="K1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>8</v>
-      </c>
-      <c r="R1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S1" t="s">
-        <v>10</v>
-      </c>
-      <c r="T1" t="s">
-        <v>11</v>
-      </c>
-      <c r="U1" t="s">
-        <v>12</v>
-      </c>
-      <c r="V1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W1" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>20</v>
-      </c>
       <c r="AA1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="AB1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.55000000000000004">
@@ -2883,10 +2883,10 @@
         <v>10.11</v>
       </c>
       <c r="I2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K2">
         <v>20.194640920000001</v>
@@ -2969,10 +2969,10 @@
         <v>10.77</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K3">
         <v>20.767104861899998</v>
@@ -3055,10 +3055,10 @@
         <v>8.25</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K4">
         <v>16.764412435200001</v>
@@ -3141,10 +3141,10 @@
         <v>9.67</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K5">
         <v>15.443088515399999</v>
@@ -3221,16 +3221,16 @@
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="H6">
         <v>10.82</v>
       </c>
       <c r="I6" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J6" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K6">
         <v>18.3376402723</v>
@@ -3313,10 +3313,10 @@
         <v>8.9</v>
       </c>
       <c r="I7" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J7" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K7">
         <v>19.528554998400001</v>
@@ -3399,10 +3399,10 @@
         <v>10.82</v>
       </c>
       <c r="I8" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K8">
         <v>37.219089510000003</v>
@@ -3485,10 +3485,10 @@
         <v>11.29</v>
       </c>
       <c r="I9" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J9" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K9">
         <v>34.512036039999998</v>
@@ -3571,10 +3571,10 @@
         <v>12.44</v>
       </c>
       <c r="I10" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J10" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K10">
         <v>19.474042130000001</v>
@@ -3657,10 +3657,10 @@
         <v>9.23</v>
       </c>
       <c r="I11" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J11" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K11">
         <v>14.39202908</v>
@@ -3743,10 +3743,10 @@
         <v>10.15</v>
       </c>
       <c r="I12" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J12" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K12">
         <v>10.275180000000001</v>
@@ -3829,10 +3829,10 @@
         <v>9.36</v>
       </c>
       <c r="I13" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J13" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K13">
         <v>15.72902</v>
@@ -3915,10 +3915,10 @@
         <v>10.11</v>
       </c>
       <c r="I14" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J14" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K14">
         <v>25.2481076364</v>
@@ -4001,10 +4001,10 @@
         <v>10.77</v>
       </c>
       <c r="I15" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J15" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K15">
         <v>26.448002265100001</v>
@@ -4087,10 +4087,10 @@
         <v>8.25</v>
       </c>
       <c r="I16" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J16" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K16">
         <v>21.3768952834</v>
@@ -4173,10 +4173,10 @@
         <v>9.67</v>
       </c>
       <c r="I17" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J17" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K17">
         <v>19.046253095000001</v>
@@ -4253,16 +4253,16 @@
         <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="H18">
         <v>10.82</v>
       </c>
       <c r="I18" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J18" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K18">
         <v>23.6756831838</v>
@@ -4345,10 +4345,10 @@
         <v>8.9</v>
       </c>
       <c r="I19" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J19" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K19">
         <v>24.1489071411</v>
@@ -4431,10 +4431,10 @@
         <v>10.82</v>
       </c>
       <c r="I20" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J20" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K20">
         <v>45.115060005899998</v>
@@ -4517,10 +4517,10 @@
         <v>11.29</v>
       </c>
       <c r="I21" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J21" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K21">
         <v>48.552202651899997</v>
@@ -4603,10 +4603,10 @@
         <v>12.44</v>
       </c>
       <c r="I22" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J22" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K22">
         <v>28.832424756599998</v>
@@ -4689,10 +4689,10 @@
         <v>9.23</v>
       </c>
       <c r="I23" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J23" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K23">
         <v>17.224973680000002</v>
@@ -4775,10 +4775,10 @@
         <v>10.15</v>
       </c>
       <c r="I24" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J24" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K24">
         <v>14.673634417000001</v>
@@ -4861,10 +4861,10 @@
         <v>9.36</v>
       </c>
       <c r="I25" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J25" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K25">
         <v>17.716139580899998</v>
@@ -4947,10 +4947,10 @@
         <v>10.11</v>
       </c>
       <c r="I26" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J26" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K26">
         <v>39.603961939999998</v>
@@ -5033,10 +5033,10 @@
         <v>10.77</v>
       </c>
       <c r="I27" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J27" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K27">
         <v>42.105262760000002</v>
@@ -5119,10 +5119,10 @@
         <v>8.25</v>
       </c>
       <c r="I28" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J28" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K28">
         <v>30.349014279999999</v>
@@ -5205,10 +5205,10 @@
         <v>9.67</v>
       </c>
       <c r="I29" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J29" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K29">
         <v>30.86419678</v>
@@ -5285,16 +5285,16 @@
         <v>2</v>
       </c>
       <c r="G30" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="H30">
         <v>10.82</v>
       </c>
       <c r="I30" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J30" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K30">
         <v>45.558086400000001</v>
@@ -5377,10 +5377,10 @@
         <v>8.9</v>
       </c>
       <c r="I31" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J31" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K31">
         <v>38.610038760000002</v>
@@ -5463,10 +5463,10 @@
         <v>10.82</v>
       </c>
       <c r="I32" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J32" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K32">
         <v>73.529411319999994</v>
@@ -5549,10 +5549,10 @@
         <v>11.29</v>
       </c>
       <c r="I33" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J33" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K33">
         <v>103.62694550000001</v>
@@ -5635,10 +5635,10 @@
         <v>12.44</v>
       </c>
       <c r="I34" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J34" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K34">
         <v>56.818180079999998</v>
@@ -5721,10 +5721,10 @@
         <v>9.23</v>
       </c>
       <c r="I35" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J35" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K35">
         <v>39.920158389999997</v>
@@ -5807,10 +5807,10 @@
         <v>10.15</v>
       </c>
       <c r="I36" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J36" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K36">
         <v>26.212320330000001</v>
@@ -5893,10 +5893,10 @@
         <v>9.36</v>
       </c>
       <c r="I37" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J37" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K37">
         <v>24.906600950000001</v>
@@ -5962,8 +5962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42570B60-2586-41A4-BAE2-D8EDFEF640F8}">
   <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5974,93 +5974,93 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+      <c r="S1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" t="s">
+      <c r="T1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="U1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="V1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z1" t="s">
         <v>33</v>
       </c>
-      <c r="K1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>8</v>
-      </c>
-      <c r="R1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S1" t="s">
-        <v>10</v>
-      </c>
-      <c r="T1" t="s">
-        <v>11</v>
-      </c>
-      <c r="U1" t="s">
-        <v>12</v>
-      </c>
-      <c r="V1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W1" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>20</v>
-      </c>
       <c r="AA1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="AB1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>42811</v>
@@ -6084,10 +6084,10 @@
         <v>10.83</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K2">
         <v>55.732315161499997</v>
@@ -6146,7 +6146,7 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1">
         <v>42811</v>
@@ -6170,10 +6170,10 @@
         <v>9.58</v>
       </c>
       <c r="I3" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="K3">
         <v>16.304966901699999</v>
@@ -6232,7 +6232,7 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
         <v>42811</v>
@@ -6256,10 +6256,10 @@
         <v>10.83</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="J4" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K4">
         <v>90.497734070000007</v>
@@ -6318,7 +6318,7 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
         <v>42811</v>
@@ -6342,10 +6342,10 @@
         <v>9.58</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="K5">
         <v>24.660911559999999</v>
@@ -6404,7 +6404,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1">
         <v>42811</v>
@@ -6428,10 +6428,10 @@
         <v>10.83</v>
       </c>
       <c r="I6" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="J6" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K6">
         <v>76.001131439999995</v>
@@ -6490,7 +6490,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1">
         <v>42811</v>
@@ -6514,10 +6514,10 @@
         <v>9.58</v>
       </c>
       <c r="I7" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K7">
         <v>20.97670428</v>

</xml_diff>

<commit_message>
Clean up and anova
</commit_message>
<xml_diff>
--- a/data/MasterGlutamateSpreadsheet.xlsx
+++ b/data/MasterGlutamateSpreadsheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10788" windowHeight="8262" activeTab="5" xr2:uid="{76EBCDB3-6D80-4011-A7B4-774B8706190D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10788" windowHeight="8262" firstSheet="2" activeTab="2" xr2:uid="{76EBCDB3-6D80-4011-A7B4-774B8706190D}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeControl" sheetId="1" r:id="rId1"/>
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FCD8EB7-4592-4D74-BEC1-FD73B58EE5E9}">
   <dimension ref="A1:AB31"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView topLeftCell="I6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6042,8 +6042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42570B60-2586-41A4-BAE2-D8EDFEF640F8}">
   <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AB12" sqref="AB12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6342,58 +6342,58 @@
         <v>11</v>
       </c>
       <c r="K4">
-        <v>90.497734070000007</v>
+        <v>76.001131439999995</v>
       </c>
       <c r="L4">
-        <v>84.388183589999997</v>
+        <v>73.622925649999999</v>
       </c>
       <c r="M4">
-        <v>85.470085139999995</v>
+        <v>74.057991029999997</v>
       </c>
       <c r="N4">
-        <v>85.836906429999999</v>
+        <v>71.023647729999993</v>
       </c>
       <c r="O4">
-        <v>82.304527280000002</v>
+        <v>70.80852763</v>
       </c>
       <c r="P4">
-        <v>84.03361511</v>
+        <v>75.589738460000007</v>
       </c>
       <c r="Q4">
-        <v>96.618354800000006</v>
+        <v>83.452184299999999</v>
       </c>
       <c r="R4">
-        <v>91.743118289999998</v>
+        <v>79.998789220000006</v>
       </c>
       <c r="S4">
-        <v>96.153846740000006</v>
+        <v>79.104511639999998</v>
       </c>
       <c r="T4">
-        <v>101.0101013</v>
+        <v>79.168673709999993</v>
       </c>
       <c r="U4">
-        <v>92.592590329999993</v>
+        <v>78.399644640000005</v>
       </c>
       <c r="V4">
-        <v>89.686096190000001</v>
+        <v>76.411760119999997</v>
       </c>
       <c r="W4">
-        <v>103.0927811</v>
+        <v>84.575807359999999</v>
       </c>
       <c r="X4">
-        <v>100</v>
+        <v>82.17436447</v>
       </c>
       <c r="Y4">
-        <v>99.502487180000003</v>
+        <v>78.847509770000002</v>
       </c>
       <c r="Z4">
-        <v>97.087379459999994</v>
+        <v>79.714009480000001</v>
       </c>
       <c r="AA4">
-        <v>94.786727909999996</v>
+        <v>77.945619960000002</v>
       </c>
       <c r="AB4">
-        <v>95.693778989999998</v>
+        <v>79.060542639999994</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.55000000000000004">
@@ -6428,58 +6428,58 @@
         <v>11</v>
       </c>
       <c r="K5">
-        <v>24.660911559999999</v>
+        <v>20.97670428</v>
       </c>
       <c r="L5">
-        <v>25.157232279999999</v>
+        <v>22.55046463</v>
       </c>
       <c r="M5">
-        <v>24.906600950000001</v>
+        <v>18.66834068</v>
       </c>
       <c r="N5">
-        <v>26.007802959999999</v>
+        <v>24.36515872</v>
       </c>
       <c r="O5">
-        <v>26.881719589999999</v>
+        <v>24.707345960000001</v>
       </c>
       <c r="P5">
-        <v>27.247957230000001</v>
+        <v>24.03927358</v>
       </c>
       <c r="Q5">
-        <v>27.972028730000002</v>
+        <v>23.934946700000001</v>
       </c>
       <c r="R5">
-        <v>27.21088409</v>
+        <v>24.458878840000001</v>
       </c>
       <c r="S5">
-        <v>26.455026629999999</v>
+        <v>24.817332589999999</v>
       </c>
       <c r="T5">
-        <v>27.932960510000001</v>
+        <v>24.14574623</v>
       </c>
       <c r="U5">
-        <v>28.20874405</v>
+        <v>23.736641410000001</v>
       </c>
       <c r="V5">
-        <v>27.972028730000002</v>
+        <v>24.992215470000001</v>
       </c>
       <c r="W5">
-        <v>26.420080179999999</v>
+        <v>23.99189758</v>
       </c>
       <c r="X5">
-        <v>25.57544708</v>
+        <v>23.466433210000002</v>
       </c>
       <c r="Y5">
-        <v>25.608194350000002</v>
+        <v>22.71382268</v>
       </c>
       <c r="Z5">
-        <v>24.096385959999999</v>
+        <v>22.970566430000002</v>
       </c>
       <c r="AA5">
-        <v>26.91790009</v>
+        <v>24.416904450000001</v>
       </c>
       <c r="AB5">
-        <v>26.91790009</v>
+        <v>24.416904450000001</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.55000000000000004">
@@ -6514,58 +6514,58 @@
         <v>12</v>
       </c>
       <c r="K6">
-        <v>76.001131439999995</v>
+        <v>90.497734070000007</v>
       </c>
       <c r="L6">
-        <v>73.622925649999999</v>
+        <v>84.388183589999997</v>
       </c>
       <c r="M6">
-        <v>74.057991029999997</v>
+        <v>85.470085139999995</v>
       </c>
       <c r="N6">
-        <v>71.023647729999993</v>
+        <v>85.836906429999999</v>
       </c>
       <c r="O6">
-        <v>70.80852763</v>
+        <v>82.304527280000002</v>
       </c>
       <c r="P6">
-        <v>75.589738460000007</v>
+        <v>84.03361511</v>
       </c>
       <c r="Q6">
-        <v>83.452184299999999</v>
+        <v>96.618354800000006</v>
       </c>
       <c r="R6">
-        <v>79.998789220000006</v>
+        <v>91.743118289999998</v>
       </c>
       <c r="S6">
-        <v>79.104511639999998</v>
+        <v>96.153846740000006</v>
       </c>
       <c r="T6">
-        <v>79.168673709999993</v>
+        <v>101.0101013</v>
       </c>
       <c r="U6">
-        <v>78.399644640000005</v>
+        <v>92.592590329999993</v>
       </c>
       <c r="V6">
-        <v>76.411760119999997</v>
+        <v>89.686096190000001</v>
       </c>
       <c r="W6">
-        <v>84.575807359999999</v>
+        <v>103.0927811</v>
       </c>
       <c r="X6">
-        <v>82.17436447</v>
+        <v>100</v>
       </c>
       <c r="Y6">
-        <v>78.847509770000002</v>
+        <v>99.502487180000003</v>
       </c>
       <c r="Z6">
-        <v>79.714009480000001</v>
+        <v>97.087379459999994</v>
       </c>
       <c r="AA6">
-        <v>77.945619960000002</v>
+        <v>94.786727909999996</v>
       </c>
       <c r="AB6">
-        <v>79.060542639999994</v>
+        <v>95.693778989999998</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.55000000000000004">
@@ -6600,58 +6600,58 @@
         <v>12</v>
       </c>
       <c r="K7">
-        <v>20.97670428</v>
+        <v>24.660911559999999</v>
       </c>
       <c r="L7">
-        <v>22.55046463</v>
+        <v>25.157232279999999</v>
       </c>
       <c r="M7">
-        <v>18.66834068</v>
+        <v>24.906600950000001</v>
       </c>
       <c r="N7">
-        <v>24.36515872</v>
+        <v>26.007802959999999</v>
       </c>
       <c r="O7">
-        <v>24.707345960000001</v>
+        <v>26.881719589999999</v>
       </c>
       <c r="P7">
-        <v>24.03927358</v>
+        <v>27.247957230000001</v>
       </c>
       <c r="Q7">
-        <v>23.934946700000001</v>
+        <v>27.972028730000002</v>
       </c>
       <c r="R7">
-        <v>24.458878840000001</v>
+        <v>27.21088409</v>
       </c>
       <c r="S7">
-        <v>24.817332589999999</v>
+        <v>26.455026629999999</v>
       </c>
       <c r="T7">
-        <v>24.14574623</v>
+        <v>27.932960510000001</v>
       </c>
       <c r="U7">
-        <v>23.736641410000001</v>
+        <v>28.20874405</v>
       </c>
       <c r="V7">
-        <v>24.992215470000001</v>
+        <v>27.972028730000002</v>
       </c>
       <c r="W7">
-        <v>23.99189758</v>
+        <v>26.420080179999999</v>
       </c>
       <c r="X7">
-        <v>23.466433210000002</v>
+        <v>25.57544708</v>
       </c>
       <c r="Y7">
-        <v>22.71382268</v>
+        <v>25.608194350000002</v>
       </c>
       <c r="Z7">
-        <v>22.970566430000002</v>
+        <v>24.096385959999999</v>
       </c>
       <c r="AA7">
-        <v>24.416904450000001</v>
+        <v>26.91790009</v>
       </c>
       <c r="AB7">
-        <v>24.416904450000001</v>
+        <v>26.91790009</v>
       </c>
     </row>
   </sheetData>
@@ -13520,7 +13520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73922CA1-B06F-4DBB-B17D-C368927A988C}">
   <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14:A19"/>
     </sheetView>
   </sheetViews>

</xml_diff>